<commit_message>
chnage logo ---working code !!!!
</commit_message>
<xml_diff>
--- a/server/output/members.xlsx
+++ b/server/output/members.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -433,70 +433,47 @@
         <v>7449085120</v>
       </c>
       <c r="C2" t="str">
-        <v>aiautomationhig@gmail.com</v>
+        <v>selvasuresh460@gmail.com</v>
       </c>
       <c r="D2" t="str">
-        <v>Wealth Manager</v>
+        <v>Health insurance advisor</v>
       </c>
       <c r="E2" t="str">
-        <v>uploads/ram_1752311161933.jpeg</v>
+        <v>uploads/ram_1752314093239.jpeg</v>
       </c>
       <c r="F2" t="str">
-        <v>1752311162001</v>
+        <v>1752314093256</v>
       </c>
       <c r="G2" t="str">
-        <v>2025-07-12T09:06:02.001Z</v>
+        <v>2025-07-12T09:54:53.256Z</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>ram</v>
+        <v>Abu Inshah</v>
       </c>
       <c r="B3" t="str">
-        <v>7449085120</v>
+        <v>9943374466</v>
       </c>
       <c r="C3" t="str">
-        <v>selvasuresh460@gmail.com</v>
+        <v>aiautomationhig@gmail.com</v>
       </c>
       <c r="D3" t="str">
-        <v>Health insurance advisor</v>
+        <v>Wealth Manager</v>
       </c>
       <c r="E3" t="str">
-        <v>uploads/ram_1752314093239.jpeg</v>
+        <v>uploads/abu_inshah_1752329088201.jpeg</v>
       </c>
       <c r="F3" t="str">
-        <v>1752314093256</v>
+        <v>1752329088240</v>
       </c>
       <c r="G3" t="str">
-        <v>2025-07-12T09:54:53.256Z</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Abu Inshah</v>
-      </c>
-      <c r="B4" t="str">
-        <v>7449085120</v>
-      </c>
-      <c r="C4" t="str">
-        <v>wealthplusacademy@gmail.com</v>
-      </c>
-      <c r="D4" t="str">
-        <v>Health insurance advisor</v>
-      </c>
-      <c r="E4" t="str">
-        <v>uploads/abu_inshah_1752314719383.jpeg</v>
-      </c>
-      <c r="F4" t="str">
-        <v>1752314719399</v>
-      </c>
-      <c r="G4" t="str">
-        <v>2025-07-12T10:05:19.399Z</v>
+        <v>2025-07-12T14:04:48.240Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add new feature responsive **Working
</commit_message>
<xml_diff>
--- a/server/output/members.xlsx
+++ b/server/output/members.xlsx
@@ -397,106 +397,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>name</v>
-      </c>
-      <c r="B1" t="str">
-        <v>phone</v>
-      </c>
-      <c r="C1" t="str">
-        <v>email</v>
-      </c>
-      <c r="D1" t="str">
-        <v>designation</v>
-      </c>
-      <c r="E1" t="str">
-        <v>photo</v>
-      </c>
-      <c r="F1" t="str">
-        <v>id</v>
-      </c>
-      <c r="G1" t="str">
-        <v>createdAt</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>ram</v>
-      </c>
-      <c r="B2" t="str">
-        <v>7449085120</v>
-      </c>
-      <c r="C2" t="str">
-        <v>selvasuresh460@gmail.com</v>
-      </c>
-      <c r="D2" t="str">
-        <v>Wealth Manager</v>
-      </c>
-      <c r="E2" t="str">
-        <v>uploads/ram_1752314093239.jpeg</v>
-      </c>
-      <c r="F2" t="str">
-        <v>1752314093256</v>
-      </c>
-      <c r="G2" t="str">
-        <v>2025-07-12T09:54:53.256Z</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Abu Inshah</v>
-      </c>
-      <c r="B3" t="str">
-        <v>9943374466</v>
-      </c>
-      <c r="C3" t="str">
-        <v>aiautomationhig@gmail.com</v>
-      </c>
-      <c r="D3" t="str">
-        <v>Wealth Manager</v>
-      </c>
-      <c r="E3" t="str">
-        <v>uploads/abu_inshah_1752329088201.jpeg</v>
-      </c>
-      <c r="F3" t="str">
-        <v>1752329088240</v>
-      </c>
-      <c r="G3" t="str">
-        <v>2025-07-12T14:04:48.240Z</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>rama</v>
-      </c>
-      <c r="B4" t="str">
-        <v>7449085120</v>
-      </c>
-      <c r="C4" t="str">
-        <v>ramasubramanian25111999@gmail.com</v>
-      </c>
-      <c r="D4" t="str">
-        <v>Health insurance advisor</v>
-      </c>
-      <c r="E4" t="str">
-        <v>uploads/rama_1752332828514.jpeg</v>
-      </c>
-      <c r="F4" t="str">
-        <v>1752332828553</v>
-      </c>
-      <c r="G4" t="str">
-        <v>2025-07-12T15:07:08.553Z</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix the route issue
</commit_message>
<xml_diff>
--- a/server/output/members.xlsx
+++ b/server/output/members.xlsx
@@ -397,13 +397,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>phone</v>
+      </c>
+      <c r="D1" t="str">
+        <v>email</v>
+      </c>
+      <c r="E1" t="str">
+        <v>designation</v>
+      </c>
+      <c r="F1" t="str">
+        <v>photo</v>
+      </c>
+      <c r="G1" t="str">
+        <v>createdAt</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>1752670313518</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Abu Inshah</v>
+      </c>
+      <c r="C2" t="str">
+        <v>7449085120</v>
+      </c>
+      <c r="D2" t="str">
+        <v>aiautomationhig@gmail.com</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Health insurance advisor,Wealth Manager</v>
+      </c>
+      <c r="F2" t="str">
+        <v>uploads/abu_inshah_1752670313452.jpeg</v>
+      </c>
+      <c r="G2" t="str">
+        <v>2025-07-16T12:51:53.518Z</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>1752671851601</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Abu Inshah</v>
+      </c>
+      <c r="C3" t="str">
+        <v>7449085120</v>
+      </c>
+      <c r="D3" t="str">
+        <v>ajai17101999@gmail.com</v>
+      </c>
+      <c r="E3" t="str">
+        <v>Health insurance advisor,Wealth Manager</v>
+      </c>
+      <c r="F3" t="str">
+        <v>uploads/abu_inshah_1752671851576.jpeg</v>
+      </c>
+      <c r="G3" t="str">
+        <v>2025-07-16T13:17:31.601Z</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>